<commit_message>
errors + automatic filling in missing values + first tests
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_noclusteringMZ.xlsx
+++ b/ConfigFiles/Config_noclusteringMZ.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="159">
   <si>
     <t xml:space="preserve">Dispa-SET Configuration File</t>
   </si>
@@ -42,6 +42,9 @@
     <t xml:space="preserve">Relative Path</t>
   </si>
   <si>
+    <t xml:space="preserve">Simulations/Simulation_CAP</t>
+  </si>
+  <si>
     <t xml:space="preserve">This section defines the output of the pre-processing (which is the input of the DispaSet solver)</t>
   </si>
   <si>
@@ -150,7 +153,7 @@
     <t xml:space="preserve">Power plant data</t>
   </si>
   <si>
-    <t xml:space="preserve">Database/PowerPlants/##/2015.csv</t>
+    <t xml:space="preserve">Database/PowerPlants/##/clustered.csv</t>
   </si>
   <si>
     <t xml:space="preserve">The path is a relative path, the current directory being the one where DispaSET.py is executed.</t>
@@ -674,11 +677,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -833,15 +836,15 @@
   </sheetPr>
   <dimension ref="A1:H152"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E67" activeCellId="0" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="25.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="43.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="3.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="16.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="15.66"/>
@@ -937,81 +940,80 @@
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="13" t="str">
-        <f aca="true">CONCATENATE("Simulations/simulationTest",TODAY())</f>
-        <v>Simulations/simulationTest43605</v>
+      <c r="C18" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="D18" s="3"/>
       <c r="H18" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="13" t="n">
+        <v>9</v>
+      </c>
+      <c r="C19" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="13" t="n">
+        <v>9</v>
+      </c>
+      <c r="C20" s="14" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="13" t="n">
+        <v>9</v>
+      </c>
+      <c r="C21" s="14" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="14" t="s">
         <v>16</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="13"/>
+        <v>16</v>
+      </c>
+      <c r="C23" s="14"/>
       <c r="D23" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1026,54 +1028,54 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C31" s="16" t="n">
         <v>42005</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C32" s="16" t="n">
-        <v>42036</v>
+        <v>42156</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="13" t="n">
+        <v>26</v>
+      </c>
+      <c r="C33" s="14" t="n">
         <v>7</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C34" s="13" t="n">
+        <v>26</v>
+      </c>
+      <c r="C34" s="14" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1095,48 +1097,48 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C47" s="14" t="s">
         <v>30</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="D47" s="3"/>
       <c r="H47" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>34</v>
       </c>
       <c r="D48" s="3"/>
       <c r="H48" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C49" s="13" t="n">
+        <v>9</v>
+      </c>
+      <c r="C49" s="14" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D49" s="3"/>
       <c r="H49" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="9" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1159,140 +1161,140 @@
     </row>
     <row r="62" s="21" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B62" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H62" s="23"/>
     </row>
     <row r="63" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C63" s="24"/>
       <c r="D63" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H63" s="23" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C64" s="25" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D64" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H64" s="23" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C65" s="25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C66" s="25"/>
       <c r="D66" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F66" s="26" t="n">
         <v>0.05</v>
       </c>
       <c r="H66" s="23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C67" s="25" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D67" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H67" s="23" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C68" s="25" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D68" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H68" s="23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C69" s="25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D69" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>5</v>
@@ -1300,7 +1302,7 @@
       <c r="C70" s="25"/>
       <c r="D70" s="15"/>
       <c r="E70" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F70" s="26" t="n">
         <v>3</v>
@@ -1308,19 +1310,19 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C71" s="25" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F71" s="26" t="n">
         <v>11</v>
@@ -1328,42 +1330,42 @@
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C72" s="25" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D72" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F72" s="26" t="n">
         <v>20</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C73" s="25" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D73" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F73" s="26" t="n">
         <v>35</v>
@@ -1371,19 +1373,19 @@
     </row>
     <row r="74" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C74" s="25" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F74" s="26" t="n">
         <v>37</v>
@@ -1391,19 +1393,19 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C75" s="25" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F75" s="26" t="n">
         <v>7</v>
@@ -1411,33 +1413,33 @@
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C76" s="25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D76" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C77" s="25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D77" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F77" s="26" t="n">
         <v>8</v>
@@ -1445,17 +1447,17 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C78" s="25"/>
       <c r="D78" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F78" s="26" t="n">
         <v>0</v>
@@ -1463,14 +1465,14 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C79" s="25"/>
       <c r="D79" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="2.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1485,25 +1487,25 @@
     <row r="86" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="87" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B87" s="27"/>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B88" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="C88" s="13" t="n">
+        <v>79</v>
+      </c>
+      <c r="C88" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E88" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="F88" s="13" t="n">
+        <v>80</v>
+      </c>
+      <c r="F88" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1511,16 +1513,16 @@
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="6"/>
       <c r="B89" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="C89" s="13" t="n">
+        <v>81</v>
+      </c>
+      <c r="C89" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E89" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="F89" s="13" t="n">
+        <v>82</v>
+      </c>
+      <c r="F89" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1528,16 +1530,16 @@
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="6"/>
       <c r="B90" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="C90" s="13" t="n">
+        <v>83</v>
+      </c>
+      <c r="C90" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E90" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="F90" s="13" t="n">
+        <v>84</v>
+      </c>
+      <c r="F90" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1545,16 +1547,16 @@
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="6"/>
       <c r="B91" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="C91" s="13" t="n">
+        <v>85</v>
+      </c>
+      <c r="C91" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E91" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="F91" s="13" t="n">
+        <v>86</v>
+      </c>
+      <c r="F91" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1562,16 +1564,16 @@
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="6"/>
       <c r="B92" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="C92" s="13" t="n">
+        <v>87</v>
+      </c>
+      <c r="C92" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E92" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="F92" s="13" t="n">
+        <v>88</v>
+      </c>
+      <c r="F92" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1579,16 +1581,16 @@
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="6"/>
       <c r="B93" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="C93" s="13" t="n">
+        <v>89</v>
+      </c>
+      <c r="C93" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E93" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="F93" s="13" t="n">
+        <v>90</v>
+      </c>
+      <c r="F93" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1596,16 +1598,16 @@
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="6"/>
       <c r="B94" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="C94" s="13" t="n">
+        <v>91</v>
+      </c>
+      <c r="C94" s="14" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E94" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="F94" s="13" t="n">
+        <v>92</v>
+      </c>
+      <c r="F94" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1613,16 +1615,16 @@
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="6"/>
       <c r="B95" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="C95" s="13" t="n">
+        <v>93</v>
+      </c>
+      <c r="C95" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E95" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="F95" s="13" t="n">
+        <v>94</v>
+      </c>
+      <c r="F95" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1630,16 +1632,16 @@
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="6"/>
       <c r="B96" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="C96" s="13" t="n">
+        <v>95</v>
+      </c>
+      <c r="C96" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E96" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="F96" s="13" t="n">
+        <v>96</v>
+      </c>
+      <c r="F96" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1647,16 +1649,16 @@
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="6"/>
       <c r="B97" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="C97" s="13" t="n">
+        <v>97</v>
+      </c>
+      <c r="C97" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E97" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="F97" s="13" t="n">
+        <v>98</v>
+      </c>
+      <c r="F97" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1664,16 +1666,16 @@
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="6"/>
       <c r="B98" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="C98" s="13" t="n">
+        <v>99</v>
+      </c>
+      <c r="C98" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E98" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="F98" s="13" t="n">
+        <v>100</v>
+      </c>
+      <c r="F98" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1681,16 +1683,16 @@
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="6"/>
       <c r="B99" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="C99" s="13" t="n">
+        <v>101</v>
+      </c>
+      <c r="C99" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E99" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="F99" s="13" t="n">
+        <v>102</v>
+      </c>
+      <c r="F99" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1698,16 +1700,16 @@
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="6"/>
       <c r="B100" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="C100" s="13" t="n">
+        <v>103</v>
+      </c>
+      <c r="C100" s="14" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E100" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="F100" s="13" t="n">
+        <v>104</v>
+      </c>
+      <c r="F100" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1715,14 +1717,14 @@
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="6"/>
       <c r="B101" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="C101" s="13" t="n">
+        <v>105</v>
+      </c>
+      <c r="C101" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E101" s="28" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F101" s="26" t="n">
         <f aca="false">FALSE()</f>
@@ -1732,14 +1734,14 @@
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="6"/>
       <c r="B102" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="C102" s="13" t="n">
+        <v>107</v>
+      </c>
+      <c r="C102" s="14" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E102" s="28" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F102" s="26" t="n">
         <f aca="false">FALSE()</f>
@@ -1758,15 +1760,15 @@
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C112" s="26" t="n">
         <v>1</v>
@@ -1774,38 +1776,38 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B113" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="C113" s="26" t="n">
         <v>1</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C114" s="26" t="n">
         <v>1</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C115" s="26" t="n">
         <v>1</v>
@@ -1829,12 +1831,12 @@
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="29" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C132" s="30" t="n">
         <f aca="false">TRUE()</f>
@@ -1843,7 +1845,7 @@
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="29" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C133" s="30" t="n">
         <f aca="false">TRUE()</f>
@@ -1852,7 +1854,7 @@
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="29" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C134" s="30" t="n">
         <f aca="false">TRUE()</f>
@@ -1861,7 +1863,7 @@
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B135" s="29" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C135" s="30" t="n">
         <f aca="false">FALSE()</f>
@@ -1870,7 +1872,7 @@
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="29" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C136" s="30" t="n">
         <f aca="false">TRUE()</f>
@@ -1879,7 +1881,7 @@
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="29" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C137" s="30" t="n">
         <f aca="false">TRUE()</f>
@@ -1888,7 +1890,7 @@
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="29" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C138" s="30" t="n">
         <f aca="false">FALSE()</f>
@@ -1897,7 +1899,7 @@
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="29" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C139" s="30" t="n">
         <f aca="false">FALSE()</f>
@@ -1906,7 +1908,7 @@
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="29" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C140" s="30" t="n">
         <f aca="false">FALSE()</f>
@@ -1915,7 +1917,7 @@
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="29" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C141" s="30" t="n">
         <f aca="false">FALSE()</f>
@@ -1924,7 +1926,7 @@
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="29" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C142" s="30" t="n">
         <f aca="false">TRUE()</f>
@@ -1933,7 +1935,7 @@
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="29" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C143" s="30" t="n">
         <f aca="false">TRUE()</f>
@@ -1942,7 +1944,7 @@
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="29" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C144" s="30" t="n">
         <f aca="false">TRUE()</f>
@@ -1951,7 +1953,7 @@
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="29" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C145" s="30" t="n">
         <f aca="false">FALSE()</f>
@@ -1960,7 +1962,7 @@
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="29" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C146" s="30" t="n">
         <f aca="false">FALSE()</f>
@@ -1973,12 +1975,12 @@
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B152" s="29" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C152" s="30" t="n">
         <f aca="false">TRUE()</f>
@@ -2118,16 +2120,16 @@
   <sheetData>
     <row r="1" s="31" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="31" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2136,13 +2138,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2151,31 +2153,31 @@
         <v>0</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2208,51 +2210,51 @@
   <sheetData>
     <row r="1" s="31" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="31" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G1" s="31" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J1" s="31" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="K1" s="31" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="L1" s="31" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="M1" s="31" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="N1" s="31" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="O1" s="31" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="31" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B2" s="32" t="n">
         <f aca="false">TRUE()</f>
@@ -2313,7 +2315,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="31" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B3" s="32" t="n">
         <f aca="false">TRUE()</f>
@@ -2374,7 +2376,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="31" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B4" s="32" t="n">
         <f aca="false">FALSE()</f>
@@ -2435,7 +2437,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="31" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B5" s="32" t="n">
         <f aca="false">FALSE()</f>
@@ -2496,7 +2498,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B6" s="32" t="n">
         <f aca="false">TRUE()</f>
@@ -2557,7 +2559,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="31" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B7" s="32" t="n">
         <f aca="false">TRUE()</f>
@@ -2618,7 +2620,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="31" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B8" s="32" t="n">
         <f aca="false">FALSE()</f>
@@ -2679,7 +2681,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="31" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B9" s="32" t="n">
         <f aca="false">FALSE()</f>
@@ -2740,7 +2742,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="31" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B10" s="32" t="n">
         <f aca="false">FALSE()</f>
@@ -2801,7 +2803,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="31" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B11" s="32" t="n">
         <f aca="false">FALSE()</f>
@@ -2862,7 +2864,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="31" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B12" s="32" t="n">
         <f aca="false">TRUE()</f>
@@ -2923,7 +2925,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="31" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B13" s="32" t="n">
         <f aca="false">TRUE()</f>
@@ -2984,7 +2986,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="31" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B14" s="32" t="n">
         <f aca="false">TRUE()</f>
@@ -3045,7 +3047,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="31" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B15" s="32" t="n">
         <f aca="false">FALSE()</f>
@@ -3106,7 +3108,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="31" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B16" s="32" t="n">
         <f aca="false">FALSE()</f>

</xml_diff>